<commit_message>
Some of Hybrid Framework file(TestComplete)
</commit_message>
<xml_diff>
--- a/ConfigurationSheet.xlsx
+++ b/ConfigurationSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="735" windowWidth="20115" windowHeight="7335"/>
+    <workbookView xWindow="240" yWindow="735" windowWidth="20115" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
   <si>
     <t>App_Name</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>http://www.travelex.co.uk.rgt.salt/gb/widget/currency</t>
-  </si>
-  <si>
-    <t>RGT_AUSCountry</t>
   </si>
 </sst>
 </file>
@@ -239,7 +236,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -441,10 +438,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -478,6 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="16" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="16" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
@@ -822,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,7 +851,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1028,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1409,29 +1407,14 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="19">
-        <v>10</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
@@ -1451,10 +1434,9 @@
     <hyperlink ref="C14" r:id="rId9"/>
     <hyperlink ref="C8" r:id="rId10"/>
     <hyperlink ref="C15" r:id="rId11"/>
-    <hyperlink ref="C16" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>